<commit_message>
Adds FF55 scenario with road CO2 standard effects integrated; uses FoPITY-2. Assumes - no PHEVs sold after 2035 (align with LDV 100% CO2 reduction); - 3% annual fuel economy improvements for ICE buses & trucks (to align with ICCT HDV study); and - H2 vehicles do not qualify as ZEVs (to align with ICCT HDV study)
</commit_message>
<xml_diff>
--- a/InputData/trans/VTQaZ/Veh Techs Qualifying as ZEVs.xlsx
+++ b/InputData/trans/VTQaZ/Veh Techs Qualifying as ZEVs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\VTQaZ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\trans\VTQaZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2410B116-F72B-481A-8955-3426D2F171F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7028812-4CBD-4571-BFF4-0E3943613A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{7166B4F5-29DF-47A7-8501-7E54D22AC689}"/>
+    <workbookView xWindow="58950" yWindow="3855" windowWidth="25500" windowHeight="13185" activeTab="1" xr2:uid="{7166B4F5-29DF-47A7-8501-7E54D22AC689}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -143,9 +143,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -183,7 +183,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -289,7 +289,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -431,7 +431,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -441,16 +441,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C5140B-A3FA-4DAF-B6D3-27BA9BD40705}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -471,16 +471,16 @@
   </sheetPr>
   <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6:AF6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -578,7 +578,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -676,7 +676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -774,7 +774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -872,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -970,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1166,102 +1166,102 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reverts LDV VTQaZ so PHEVs don't qualify from 2035
</commit_message>
<xml_diff>
--- a/InputData/trans/VTQaZ/Veh Techs Qualifying as ZEVs.xlsx
+++ b/InputData/trans/VTQaZ/Veh Techs Qualifying as ZEVs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\trans\VTQaZ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\trans\VTQaZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD75852-D3EB-4C85-B99A-5F9A026D83F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A0CEA5-A797-464D-B9C0-ECAF70B8F0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{7166B4F5-29DF-47A7-8501-7E54D22AC689}"/>
+    <workbookView xWindow="32055" yWindow="1740" windowWidth="22245" windowHeight="14595" activeTab="1" xr2:uid="{7166B4F5-29DF-47A7-8501-7E54D22AC689}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -446,18 +446,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C5140B-A3FA-4DAF-B6D3-27BA9BD40705}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,16 +478,16 @@
   </sheetPr>
   <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6:AF6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -585,7 +585,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -781,7 +781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -879,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1027,55 +1027,55 @@
         <v>1</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1287,12 +1287,12 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2092,12 +2092,12 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2897,12 +2897,12 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -3702,12 +3702,12 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -4507,12 +4507,12 @@
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4708,7 +4708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>

</xml_diff>